<commit_message>
Finish admin for rinkeby
</commit_message>
<xml_diff>
--- a/public/assets/Sample.xlsx
+++ b/public/assets/Sample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Develop/Workspace/Blockchain/Trustswap/trustswap-vest-admin-ui/public/assets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C96BBA64-77BF-DF4F-93C8-6D13532CB29B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2B843C-F7D4-274E-B44E-6B502D355F61}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{80D4C309-0B11-6749-9F62-84746EF6F9CD}"/>
+    <workbookView xWindow="5460" yWindow="1740" windowWidth="28040" windowHeight="17440" xr2:uid="{80D4C309-0B11-6749-9F62-84746EF6F9CD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Address</t>
   </si>
@@ -45,19 +45,31 @@
     <t>0xAA1D9000dDdC91227ef748C9389cB90bc9D355cF</t>
   </si>
   <si>
-    <t>0x8875200B445d72a2633a0a6a3673Ae046e9E4b1b</t>
-  </si>
-  <si>
-    <t>0xFbD7AB8F92b6Cb85c61ad5917C8fcb71b907c679</t>
-  </si>
-  <si>
-    <t>1D</t>
-  </si>
-  <si>
     <t>5H</t>
   </si>
   <si>
     <t>3M</t>
+  </si>
+  <si>
+    <t>StartTime</t>
+  </si>
+  <si>
+    <t>2D</t>
+  </si>
+  <si>
+    <t>Immediately</t>
+  </si>
+  <si>
+    <t>5W</t>
+  </si>
+  <si>
+    <t>0x410da55D45bE4f9e0616F2a1Cac7917d1baB92e5</t>
+  </si>
+  <si>
+    <t>0xFc3BD8d2F74262B4dc52904cDce974822AA812bF</t>
+  </si>
+  <si>
+    <t>0xEDAAb775b37A5f5098390A1e5bA2e3f6B423AE7b</t>
   </si>
 </sst>
 </file>
@@ -93,8 +105,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,73 +427,105 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42855C4D-F2AA-7941-9C72-3C161254EA3E}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47.1640625" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2">
+        <v>44214.333333333336</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="D2" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3">
+      <c r="B3" s="2">
+        <v>44215.723611111112</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>44217.333333333336</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="D4" s="1">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="2">
+        <v>44257.305555555555</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>5000</v>
-      </c>
+      <c r="C6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
+        <v>70000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>